<commit_message>
Update SRS Document and Gantt Chart
</commit_message>
<xml_diff>
--- a/SRS/Bảng phân công công việc.xlsx
+++ b/SRS/Bảng phân công công việc.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Phân tích</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">Mô tả yêu cầu phần mềm
 </t>
@@ -40,45 +37,70 @@
 phi chức năng</t>
   </si>
   <si>
+    <t>Xác định Use Case</t>
+  </si>
+  <si>
+    <t>BẢNG PHÂN CÔNG CÔNG VIỆC</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Chi tiết công việc</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Thành viên</t>
+  </si>
+  <si>
+    <t>Tuần 1</t>
+  </si>
+  <si>
+    <t>Đặc tả use case</t>
+  </si>
+  <si>
+    <t>Use Case: Tìm kiếm phòng, Đặt phòng</t>
+  </si>
+  <si>
+    <t>Trần Thị Ngọc Hân</t>
+  </si>
+  <si>
     <t>Huỳnh Trọng Tuấn
-Trần Thị Ngọc Hân</t>
-  </si>
-  <si>
-    <t>Xác định Use Case</t>
-  </si>
-  <si>
-    <t>Hồ Thanh Hiệp
+Hồ Thanh Hiệp</t>
+  </si>
+  <si>
+    <t>Github
+Outline SRS Document</t>
+  </si>
+  <si>
+    <t>Phân tích yêu cầu</t>
+  </si>
+  <si>
+    <t>Trần Thị Ngọc Hân
 Phạm Đức Hiếu</t>
   </si>
   <si>
-    <t>BẢNG PHÂN CÔNG CÔNG VIỆC</t>
-  </si>
-  <si>
-    <t>Công việc</t>
-  </si>
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Chi tiết công việc</t>
-  </si>
-  <si>
-    <t>Thời gian</t>
-  </si>
-  <si>
-    <t>Thành viên</t>
-  </si>
-  <si>
-    <t>Tuần 1</t>
-  </si>
-  <si>
-    <t>Đặc tả use case</t>
-  </si>
-  <si>
-    <t>Use Case: Tìm kiếm phòng, Đặt phòng</t>
-  </si>
-  <si>
-    <t>Trần Thị Ngọc Hân</t>
+    <t>Tuần 2, 3</t>
+  </si>
+  <si>
+    <t>UML Design (Activity Diagram,Sequence Diagram)</t>
+  </si>
+  <si>
+    <t>Use Case: Đăng nhập, Đăng xuất, Thanh toán</t>
+  </si>
+  <si>
+    <t>Use Case: Quản lý đặt phòng</t>
+  </si>
+  <si>
+    <t>Use Case: Quản lý phòng</t>
+  </si>
+  <si>
+    <t>Use Case: Quản lý khách hàng</t>
   </si>
 </sst>
 </file>
@@ -126,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -254,6 +282,52 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -262,27 +336,89 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -290,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -310,9 +446,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -325,34 +458,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,143 +801,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="3" max="3" width="45.44140625" customWidth="1"/>
     <col min="4" max="4" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="30">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="30"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19">
+        <v>3</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="19"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
         <v>4</v>
       </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
-        <v>2</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="E3:E11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="E12:E15"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Use sase: Quan lý khách hàng
Use sase: Quan lý khách hàng
</commit_message>
<xml_diff>
--- a/SRS/Bảng phân công công việc.xlsx
+++ b/SRS/Bảng phân công công việc.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HDs\Desktop\DACNPM\DACN_CongNghePhanMem\SRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh Hiep\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5448"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">Mô tả yêu cầu phần mềm
 </t>
@@ -101,13 +101,16 @@
   </si>
   <si>
     <t>Use Case: Quản lý khách hàng</t>
+  </si>
+  <si>
+    <t>Hồ Thanh Hiệp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,35 +119,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -426,100 +423,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,201 +790,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="16" customFormat="1" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30">
+    <row r="4" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26">
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="30"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
       <c r="B5" s="28"/>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
       <c r="B6" s="29"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
         <v>3</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="5" t="s">
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="5" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="21" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>4</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="31" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="32"/>
-    </row>
-    <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="32"/>
-    </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="33"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+    <row r="13" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Update Bảng phân công công việc.xlsx
</commit_message>
<xml_diff>
--- a/SRS/Bảng phân công công việc.xlsx
+++ b/SRS/Bảng phân công công việc.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HDs\Desktop\DACNPM\DACN_CongNghePhanMem\SRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACN_CongNghePhanMem\SRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5448"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,26 +493,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,28 +796,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -834,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -849,11 +849,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+    <row r="4" spans="1:5" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -864,9 +864,9 @@
       </c>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
+    <row r="5" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -875,9 +875,9 @@
       </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:5" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
-      <c r="B6" s="29"/>
+    <row r="6" spans="1:5" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
@@ -886,11 +886,11 @@
       </c>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+    <row r="7" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
         <v>3</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -901,9 +901,9 @@
       </c>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
-      <c r="B8" s="28"/>
+    <row r="8" spans="1:5" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
@@ -912,9 +912,9 @@
       </c>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-      <c r="B9" s="28"/>
+    <row r="9" spans="1:5" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
@@ -923,9 +923,9 @@
       </c>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="28"/>
+    <row r="10" spans="1:5" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
@@ -934,9 +934,9 @@
       </c>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28"/>
+    <row r="11" spans="1:5" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="11" t="s">
         <v>23</v>
       </c>
@@ -945,7 +945,7 @@
       </c>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>4</v>
       </c>
@@ -958,42 +958,42 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="21"/>
       <c r="C13" s="12"/>
       <c r="D13" s="14"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="21"/>
       <c r="C14" s="12"/>
       <c r="D14" s="14"/>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="22"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>

</xml_diff>